<commit_message>
turnos ordenados, marketing turno
</commit_message>
<xml_diff>
--- a/turnos.xlsx
+++ b/turnos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b68001cfe7d3a722/Ambiente de Trabalho/jeec/schedule_otimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{51869039-E702-4671-BD02-74778DF24566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D87ED42D-5C39-4BD0-9412-0A82205798FE}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{51869039-E702-4671-BD02-74778DF24566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFEA1A22-5D3D-4181-B504-43AE04512CAC}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12216" xr2:uid="{0784EA88-8875-478A-91C5-C3F582E7D373}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0784EA88-8875-478A-91C5-C3F582E7D373}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -157,6 +157,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -459,7 +463,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A5" sqref="A5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -486,69 +490,69 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
       <c r="C2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -556,13 +560,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
@@ -570,30 +574,30 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>